<commit_message>
updated specs to call all method less often - less 'let' instances
</commit_message>
<xml_diff>
--- a/Classes_exaplained.xlsx
+++ b/Classes_exaplained.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="27260" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="27360" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -825,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2215,5 +2215,6 @@
     <mergeCell ref="J24:P24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>